<commit_message>
Updated TestDescriptors Test Case
</commit_message>
<xml_diff>
--- a/TestData/AccountNumbers.xlsx
+++ b/TestData/AccountNumbers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UIPath\VPSAutomation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E63BF1-2BB3-4D2F-A239-31FC56A828D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{027C2F98-BC28-4B4F-AC7C-69198BC387DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25935" yWindow="3270" windowWidth="24525" windowHeight="14010" xr2:uid="{489EF063-A50C-4174-A25E-056DA4E3CD9F}"/>
+    <workbookView xWindow="-26685" yWindow="3495" windowWidth="24525" windowHeight="14010" xr2:uid="{489EF063-A50C-4174-A25E-056DA4E3CD9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated VT Test Case to include Verification Point.
</commit_message>
<xml_diff>
--- a/TestData/AccountNumbers.xlsx
+++ b/TestData/AccountNumbers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UIPath\VPSAutomation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{027C2F98-BC28-4B4F-AC7C-69198BC387DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F367508-0A21-440C-83F4-BDF259E7E789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26685" yWindow="3495" windowWidth="24525" windowHeight="14010" xr2:uid="{489EF063-A50C-4174-A25E-056DA4E3CD9F}"/>
+    <workbookView xWindow="-26610" yWindow="3450" windowWidth="24525" windowHeight="14010" xr2:uid="{489EF063-A50C-4174-A25E-056DA4E3CD9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Name</t>
   </si>
@@ -53,7 +53,43 @@
     <t>Result</t>
   </si>
   <si>
-    <t>Pass</t>
+    <t>DateTime</t>
+  </si>
+  <si>
+    <t>Execute</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Anhu Kirty</t>
+  </si>
+  <si>
+    <t>365289</t>
+  </si>
+  <si>
+    <t>Kuimy Awecrt</t>
+  </si>
+  <si>
+    <t>145239</t>
+  </si>
+  <si>
+    <t>lokiju mveux</t>
+  </si>
+  <si>
+    <t>589612</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>02/23/2024 23:12:49</t>
+  </si>
+  <si>
+    <t>02/23/2024 23:13:01</t>
+  </si>
+  <si>
+    <t>02/23/2024 23:13:08</t>
   </si>
 </sst>
 </file>
@@ -77,7 +113,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -85,12 +121,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,50 +459,101 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2D2FC87-670B-4AD9-9317-62BCB3FFA6AB}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="C2" s="1">
         <v>584789</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="C3" s="1">
         <v>359621</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>